<commit_message>
add missing treatment add min and max
</commit_message>
<xml_diff>
--- a/#1323 1342 Result Range of Preservation Index 8-14-14.xlsx
+++ b/#1323 1342 Result Range of Preservation Index 8-14-14.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="30">
   <si>
     <t>Scenario #</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Full Depth Reclamation</t>
+  </si>
+  <si>
+    <t>HMA Thin Overlay - Preventive</t>
   </si>
 </sst>
 </file>
@@ -236,17 +239,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -259,11 +253,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,904 +586,974 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="23.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="21">
         <v>1342</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="26"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="24"/>
-      <c r="B5" s="28" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28" t="s">
+      <c r="C5" s="24">
+        <f>MIN(C6:C12)</f>
+        <v>-4.9200000000000001E-2</v>
+      </c>
+      <c r="D5" s="24">
+        <f>MAX(D6:D12)</f>
+        <v>27.130400000000002</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="G5" s="24">
+        <f>MIN(G6:G12)</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H5" s="24">
+        <f>MAX(H6:H12)</f>
+        <v>90.909300000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="24">
+      <c r="A6" s="21">
         <v>1</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="21">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>3.3854000000000002</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>1</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="21">
         <v>0.39179999999999998</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>4.9390999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="24">
+      <c r="A7" s="21">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="21">
         <v>4.1999000000000004</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <v>4.3318000000000003</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="21">
         <v>2</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="21">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <v>3.6900000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="24">
+      <c r="A8" s="21">
         <v>3</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="21">
         <v>0</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>0</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>3</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="21">
         <v>0.13819999999999999</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="21">
         <v>0.94679999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="24">
+      <c r="A9" s="21">
         <v>4</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="21">
         <v>2.6700000000000002E-2</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>27.130400000000002</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>4</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="24">
-        <v>5</v>
-      </c>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="21">
+        <v>5</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="21">
         <v>0.32479999999999998</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>0.32479999999999998</v>
       </c>
-      <c r="E10" s="24">
-        <v>5</v>
-      </c>
-      <c r="F10" s="24" t="s">
+      <c r="E10" s="21">
+        <v>5</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <v>6.9599999999999995E-2</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>90.909300000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="24">
-        <v>6</v>
-      </c>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="21">
+        <v>6</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="21">
         <v>-4.9200000000000001E-2</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>2.35E-2</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="E11" s="21">
+        <v>6</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0.94930000000000003</v>
+      </c>
+      <c r="H11" s="21">
+        <v>2.8719999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="A12" s="21">
+        <v>7</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="21">
+        <v>0.34649999999999997</v>
+      </c>
+      <c r="D12" s="21">
+        <v>0.36609999999999998</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="27"/>
-      <c r="B14" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="24"/>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="28" t="s">
+      <c r="C15" s="24">
+        <f>MIN(C16:C24)</f>
+        <v>-0.54339999999999999</v>
+      </c>
+      <c r="D15" s="24">
+        <f>MAX(D16:D23)</f>
+        <v>80.343699999999998</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="24">
+        <f>MIN(G16:G23)</f>
+        <v>-0.30170000000000002</v>
+      </c>
+      <c r="H15" s="24">
+        <f>MAX(H16:H23)</f>
+        <v>1.7181999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="24">
+      <c r="A16" s="21">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="21">
         <v>0.32369999999999999</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>0.3453</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>1</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <v>0.28249999999999997</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="21">
         <v>0.87390000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="24">
+      <c r="A17" s="21">
         <v>2</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="21">
         <v>0.28920000000000001</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="21">
         <v>1.0846</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <v>2</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="21">
         <v>7.3700000000000002E-2</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="21">
         <v>0.31080000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="24">
+      <c r="A18" s="21">
         <v>3</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="21">
         <v>0.17960000000000001</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>0.21540000000000001</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>3</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="21">
         <v>7.2599999999999998E-2</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="21">
         <v>1.3737999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="24">
+      <c r="A19" s="21">
         <v>4</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="21">
         <v>6.6900000000000001E-2</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="21">
         <v>4.26</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="21">
         <v>4</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="21">
         <v>-0.24690000000000001</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="21">
         <v>1.7181999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="24">
-        <v>5</v>
-      </c>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="21">
+        <v>5</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="21">
         <v>-0.54339999999999999</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="21">
         <v>80.343699999999998</v>
       </c>
-      <c r="E20" s="24">
-        <v>5</v>
-      </c>
-      <c r="F20" s="24" t="s">
+      <c r="E20" s="21">
+        <v>5</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="21">
         <v>-0.30170000000000002</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="21">
         <v>1.3888</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="24">
-        <v>6</v>
-      </c>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="21">
+        <v>6</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="21">
         <v>0.15809999999999999</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="21">
         <v>1.3098000000000001</v>
       </c>
-      <c r="E21" s="24">
-        <v>6</v>
-      </c>
-      <c r="F21" s="24" t="s">
+      <c r="E21" s="21">
+        <v>6</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24">
+      <c r="A22" s="21">
         <v>7</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="21">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="21">
         <v>0.77780000000000005</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="21">
         <v>7</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="24">
+      <c r="A23" s="21">
         <v>8</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="21">
         <v>-9.2999999999999992E-3</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="21">
         <v>0.5343</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="21">
         <v>8</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="21">
         <v>-1E-4</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="21">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24">
+      <c r="A24" s="21">
         <v>9</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="26.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="14">
         <v>1342</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17" t="s">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="18"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21">
+      <c r="C30" s="24">
+        <f>MIN(C31:C38)</f>
+        <v>0.17219999999999999</v>
+      </c>
+      <c r="D30" s="24">
+        <f>MAX(D31:D38)</f>
+        <v>8.7696000000000005</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="17">
+        <f>MIN(G31:G36)</f>
+        <v>0.2356</v>
+      </c>
+      <c r="H30" s="17">
+        <f>MAX(H31:H36)</f>
+        <v>6.3913000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="14">
         <v>1</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="B31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="18">
+        <v>1</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="14">
         <v>2</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="16">
+      <c r="B32" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="14">
+        <v>3</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="18">
+        <v>3</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="14">
+        <v>0.32519999999999999</v>
+      </c>
+      <c r="H33" s="14">
+        <v>5.1539000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="14">
+        <v>4</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="18">
+        <v>4</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="14">
+        <v>5</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="18">
+        <v>5</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="14">
+        <v>0.2356</v>
+      </c>
+      <c r="H35" s="14">
+        <v>2.2078000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="14">
+        <v>6</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="18">
+        <v>6</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="14">
+        <v>0.40870000000000001</v>
+      </c>
+      <c r="H36" s="14">
+        <v>6.3913000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="14">
+        <v>7</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="20">
+        <v>0.2152</v>
+      </c>
+      <c r="D37" s="20">
+        <v>8.7696000000000005</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="14">
+        <v>8</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="14">
+        <v>0.17219999999999999</v>
+      </c>
+      <c r="D38" s="14">
+        <v>4.5782999999999996</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="16"/>
+      <c r="B39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="26"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="14"/>
+      <c r="B40" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="17">
+        <f>MIN(C41:C49)</f>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="D40" s="17">
+        <f>MAX(D41:D49)</f>
+        <v>2.9552</v>
+      </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="17">
+        <f>MIN(G41:G49)</f>
+        <v>0.1028</v>
+      </c>
+      <c r="H40" s="17">
+        <f>MAX(H41:H49)</f>
+        <v>1.3105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="14">
         <v>1</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B41" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="21">
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14">
+        <v>1</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="14">
+        <v>0.91169999999999995</v>
+      </c>
+      <c r="H41" s="14">
+        <v>1.0504</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="14">
         <v>2</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="16">
+      <c r="C42" s="14">
+        <v>0.33950000000000002</v>
+      </c>
+      <c r="D42" s="14">
+        <v>2.2454000000000001</v>
+      </c>
+      <c r="E42" s="14">
         <v>2</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="21">
+      <c r="F42" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="14">
         <v>3</v>
       </c>
-      <c r="F32" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="16">
+      <c r="B43" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="14">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="D43" s="14">
+        <v>2.9552</v>
+      </c>
+      <c r="E43" s="14">
         <v>3</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="21">
+      <c r="F43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="14">
         <v>4</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="B44" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="14">
+        <v>0.1908</v>
+      </c>
+      <c r="D44" s="14">
+        <v>2.0004</v>
+      </c>
+      <c r="E44" s="14">
+        <v>4</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="14">
+        <v>0.1028</v>
+      </c>
+      <c r="H44" s="14">
+        <v>0.2492</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="14">
+        <v>5</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="14">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D45" s="14">
+        <v>0.50319999999999998</v>
+      </c>
+      <c r="E45" s="14">
+        <v>5</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="14">
+        <v>0.2278</v>
+      </c>
+      <c r="H45" s="14">
+        <v>0.40379999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="14">
+        <v>6</v>
+      </c>
+      <c r="B46" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="16">
-        <v>0.32519999999999999</v>
-      </c>
-      <c r="H33" s="16">
-        <v>5.1539000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="16">
-        <v>4</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14">
+        <v>6</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="14">
+        <v>7</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14">
+        <v>7</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="14">
         <v>8</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="21">
-        <v>5</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="16">
-        <v>5</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="21">
-        <v>6</v>
-      </c>
-      <c r="F35" s="16" t="s">
+      <c r="B48" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="16">
-        <v>0.2356</v>
-      </c>
-      <c r="H35" s="16">
-        <v>2.2078000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="16">
-        <v>6</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="21">
-        <v>7</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="16">
-        <v>0.40870000000000001</v>
-      </c>
-      <c r="H36" s="16">
-        <v>6.3913000000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="16">
-        <v>7</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="23">
-        <v>0.2152</v>
-      </c>
-      <c r="D37" s="23">
-        <v>8.7696000000000005</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="19"/>
-      <c r="B39" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="18"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="16">
-        <v>1</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16">
-        <v>1</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="16">
-        <v>0.91169999999999995</v>
-      </c>
-      <c r="H41" s="16">
-        <v>1.0504</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="16">
-        <v>2</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="16">
-        <v>0.33950000000000002</v>
-      </c>
-      <c r="D42" s="16">
-        <v>2.2454000000000001</v>
-      </c>
-      <c r="E42" s="16">
-        <v>2</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="16">
-        <v>3</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="16">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="D43" s="16">
-        <v>2.9552</v>
-      </c>
-      <c r="E43" s="16">
-        <v>3</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="16">
-        <v>4</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="16">
-        <v>0.1908</v>
-      </c>
-      <c r="D44" s="16">
-        <v>2.0004</v>
-      </c>
-      <c r="E44" s="16">
-        <v>4</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="16">
-        <v>0.1028</v>
-      </c>
-      <c r="H44" s="16">
-        <v>0.2492</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="16">
-        <v>5</v>
-      </c>
-      <c r="B45" s="16" t="s">
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14">
+        <v>8</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="14">
         <v>9</v>
       </c>
-      <c r="C45" s="16">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="D45" s="16">
-        <v>0.50319999999999998</v>
-      </c>
-      <c r="E45" s="16">
-        <v>5</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" s="16">
-        <v>0.2278</v>
-      </c>
-      <c r="H45" s="16">
-        <v>0.40379999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="16">
-        <v>6</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16">
-        <v>6</v>
-      </c>
-      <c r="F46" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="16">
-        <v>7</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16">
-        <v>7</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="16">
-        <v>8</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16">
-        <v>8</v>
-      </c>
-      <c r="F48" s="16" t="s">
+      <c r="B49" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="16">
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14">
         <v>9</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16">
-        <v>9</v>
-      </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="14">
         <v>0.28129999999999999</v>
       </c>
-      <c r="H49" s="16">
+      <c r="H49" s="14">
         <v>1.3105</v>
       </c>
     </row>
@@ -1504,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1551,18 +1624,18 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="15"/>
+      <c r="C4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="29"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="15"/>
+      <c r="G4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1"/>
@@ -1759,18 +1832,18 @@
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="15"/>
+      <c r="C14" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="29"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="15"/>
+      <c r="G14" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1"/>
@@ -2051,18 +2124,18 @@
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="14"/>
+      <c r="C29" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="28"/>
       <c r="E29" s="5"/>
       <c r="F29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" s="14"/>
+      <c r="G29" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3"/>
@@ -2243,18 +2316,18 @@
       <c r="B39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="14"/>
+      <c r="C39" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="28"/>
       <c r="E39" s="5"/>
       <c r="F39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="14"/>
+      <c r="G39" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3"/>

</xml_diff>

<commit_message>
good for print now
</commit_message>
<xml_diff>
--- a/#1323 1342 Result Range of Preservation Index 8-14-14.xlsx
+++ b/#1323 1342 Result Range of Preservation Index 8-14-14.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'FINE 1342'!$A$2:$H$49</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -567,10 +570,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1142,11 +1148,11 @@
       <c r="B30" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="17">
         <f>MIN(C31:C38)</f>
         <v>0.17219999999999999</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="17">
         <f>MAX(D31:D38)</f>
         <v>8.7696000000000005</v>
       </c>
@@ -1569,7 +1575,7 @@
     <mergeCell ref="G29:H29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1578,7 +1584,7 @@
   <dimension ref="A2:H49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>